<commit_message>
filter function, layout tweaks, script fixes
</commit_message>
<xml_diff>
--- a/src/cikkek.xlsx
+++ b/src/cikkek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\designlab\zylag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE76A016-2198-4B50-B476-17728EED6242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C42E5BB-4915-4554-BEA1-0F235D619E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cikkek" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>Projekt</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Kész</t>
+  </si>
+  <si>
+    <t>web, branding, logo, uiux, case study</t>
   </si>
 </sst>
 </file>
@@ -614,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +695,7 @@
         <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -714,7 +717,7 @@
         <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -756,6 +759,9 @@
       </c>
       <c r="B11" t="s">
         <v>35</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
@@ -891,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EA60CF-272A-40E8-A79B-A8A4191DFE86}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>